<commit_message>
Various bug fixes and script completions
</commit_message>
<xml_diff>
--- a/system/leaderboard.xlsx
+++ b/system/leaderboard.xlsx
@@ -1,23 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\trevor.knight\Documents\project_1\system\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevo\OneDrive\Documents\MATLAB Projects\game_login\system\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20F7010-8A4E-4E80-8E19-919CF987B079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16440" windowHeight="7650"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="10920" xr2:uid="{5D739F84-D7D3-4EBF-8F98-0FDDB5D13AEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -32,7 +44,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -98,7 +110,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -110,7 +122,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -157,6 +169,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -192,6 +221,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -343,7 +389,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75EEEC90-21D6-4187-982B-2879BF606A5A}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>